<commit_message>
starting ship fuel using item rework
</commit_message>
<xml_diff>
--- a/ProjectManagement/Modules.xlsx
+++ b/ProjectManagement/Modules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Project Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital Archive\Game Development\Active\SpaceUnknown\ProjectManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7FB8FE-DB62-4EF4-8A7F-8CB7554D00BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A433E703-005F-4CCA-9088-2C9083BC89AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BEDA9127-5E7F-4B15-9FE0-DDF043E0E148}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Adds more cargo space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second Fuel Tank </t>
+  </si>
+  <si>
+    <t>Adds more fuel tank size</t>
   </si>
 </sst>
 </file>
@@ -118,8 +124,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FEB2121-7A05-45CF-B060-A377F5C02C18}" name="Table1" displayName="Table1" ref="B3:D5" totalsRowShown="0">
-  <autoFilter ref="B3:D5" xr:uid="{6FEB2121-7A05-45CF-B060-A377F5C02C18}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FEB2121-7A05-45CF-B060-A377F5C02C18}" name="Table1" displayName="Table1" ref="B3:D6" totalsRowShown="0">
+  <autoFilter ref="B3:D6" xr:uid="{6FEB2121-7A05-45CF-B060-A377F5C02C18}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FFCC2355-E4EE-481E-98A0-1102DD5CA9A3}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4770588D-5EDD-4D5C-B0F0-3F6FEB342485}" name="Slot Type"/>
@@ -418,7 +424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F1A7B1-2AED-43D2-A412-380A2E4306DA}">
-  <dimension ref="B3:D5"/>
+  <dimension ref="B3:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="77.85546875" customWidth="1"/>
   </cols>
@@ -470,6 +476,17 @@
       </c>
       <c r="D5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>